<commit_message>
Starts to use the new Qualis (A1-A4, B1-B4)
</commit_message>
<xml_diff>
--- a/resources/qualis/qualis-conferences-2020.xlsx
+++ b/resources/qualis/qualis-conferences-2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leomurta/workspace/perfil/resources/qualis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3F9039-A7D8-7042-AB86-542AEBE51C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F05A42F-35FF-E94E-9281-6AEED203810C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="740" windowWidth="28040" windowHeight="16680" xr2:uid="{850CD0C6-2FFC-C34F-BC1D-6AFFBA835C13}"/>
   </bookViews>
@@ -8482,13 +8482,13 @@
     <t>International Workshop on Semantic and Conceptual Issues in Geographic Information Systems</t>
   </si>
   <si>
-    <t>Sigla</t>
-  </si>
-  <si>
-    <t>Título</t>
-  </si>
-  <si>
-    <t>Estrato</t>
+    <t>sigla</t>
+  </si>
+  <si>
+    <t>titulo</t>
+  </si>
+  <si>
+    <t>estrato</t>
   </si>
 </sst>
 </file>
@@ -8945,7 +8945,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E665147-095E-2148-AD2E-34634FE1C4E8}">
   <dimension ref="A1:C1406"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
Does some adjustments in the venue names
</commit_message>
<xml_diff>
--- a/resources/qualis/qualis-conferences-2020.xlsx
+++ b/resources/qualis/qualis-conferences-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leomurta/workspace/perfil/resources/qualis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F05A42F-35FF-E94E-9281-6AEED203810C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA13E32-A751-5F4C-87C0-9047C4D45371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="740" windowWidth="28040" windowHeight="16680" xr2:uid="{850CD0C6-2FFC-C34F-BC1D-6AFFBA835C13}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4218" uniqueCount="2818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4221" uniqueCount="2822">
   <si>
     <t>AAAI</t>
   </si>
@@ -8489,6 +8489,18 @@
   </si>
   <si>
     <t>estrato</t>
+  </si>
+  <si>
+    <t>Conference on Human Factors in Computing Systems</t>
+  </si>
+  <si>
+    <t>International Conference on Optimization and Learning</t>
+  </si>
+  <si>
+    <t>OLA</t>
+  </si>
+  <si>
+    <t>NC</t>
   </si>
 </sst>
 </file>
@@ -8587,7 +8599,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -8610,11 +8622,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -8629,6 +8652,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8943,10 +8967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E665147-095E-2148-AD2E-34634FE1C4E8}">
-  <dimension ref="A1:C1406"/>
+  <dimension ref="A1:C1407"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A1395" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="C1408" sqref="C1408"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11046,7 +11070,7 @@
         <v>27</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>28</v>
+        <v>2818</v>
       </c>
       <c r="C191" s="2" t="s">
         <v>2</v>
@@ -24415,6 +24439,17 @@
       </c>
       <c r="C1406" s="2" t="s">
         <v>508</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1407" s="14" t="s">
+        <v>2820</v>
+      </c>
+      <c r="B1407" s="14" t="s">
+        <v>2819</v>
+      </c>
+      <c r="C1407" s="14" t="s">
+        <v>2821</v>
       </c>
     </row>
   </sheetData>

</xml_diff>